<commit_message>
update rooster and game data for new season
</commit_message>
<xml_diff>
--- a/data/roster.xlsx
+++ b/data/roster.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanuel.woldekidan/gitrepos/flamingo_stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829F341D-8F29-EA4B-B0F1-8C81F3CDC22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43B9413-9CCA-BD46-8F11-2C89F82E3201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="27040" xr2:uid="{09AF5A8C-78D4-2142-A69D-63FA30327E3F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>Guido</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Goncalo</t>
   </si>
 </sst>
 </file>
@@ -456,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084FA9C7-071B-744B-9071-1A20F95C2B9B}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,12 +499,12 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -532,70 +541,82 @@
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>41</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
+      <c r="A9" s="3">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>36</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>77</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C14" s="6"/>
@@ -605,6 +626,30 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>